<commit_message>
Duble magyar módszer debuggolva, üres táblázaton jól működik. Széles körű tesztelés hátra van.
</commit_message>
<xml_diff>
--- a/requests_admin.xlsx
+++ b/requests_admin.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Napok száma</t>
   </si>
@@ -39,22 +39,10 @@
     <t xml:space="preserve">NAME   #1</t>
   </si>
   <si>
-    <t xml:space="preserve">n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">é</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
     <t xml:space="preserve">NAME   #2</t>
   </si>
   <si>
     <t xml:space="preserve">NAME   #3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">É</t>
   </si>
   <si>
     <t xml:space="preserve">NAME   #4</t>
@@ -429,7 +417,7 @@
   <dimension ref="A1:AN1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -444,9 +432,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="C1" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="n">
+        <f aca="false">SUM(B4:B10)</f>
+        <v>14</v>
+      </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -492,7 +483,10 @@
       <c r="B2" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="4" t="n">
+        <f aca="false">SUM(C4:C10)</f>
+        <v>7</v>
+      </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -566,17 +560,17 @@
         <f aca="false">IF(I3="","",IF(I3+1-$B$1 &gt; 0, "", I3+1))</f>
         <v>7</v>
       </c>
-      <c r="K3" s="7" t="n">
+      <c r="K3" s="7" t="str">
         <f aca="false">IF(J3="","",IF(J3+1-$B$1 &gt; 0, "", J3+1))</f>
-        <v>8</v>
-      </c>
-      <c r="L3" s="7" t="n">
+        <v/>
+      </c>
+      <c r="L3" s="7" t="str">
         <f aca="false">IF(K3="","",IF(K3+1-$B$1 &gt; 0, "", K3+1))</f>
-        <v>9</v>
-      </c>
-      <c r="M3" s="7" t="n">
+        <v/>
+      </c>
+      <c r="M3" s="7" t="str">
         <f aca="false">IF(L3="","",IF(L3+1-$B$1 &gt; 0, "", L3+1))</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="N3" s="7" t="str">
         <f aca="false">IF(M3="","",IF(M3+1-$B$1 &gt; 0, "", M3+1))</f>
@@ -692,31 +686,21 @@
         <v>4</v>
       </c>
       <c r="B4" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>5</v>
-      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
       <c r="G4" s="10"/>
-      <c r="H4" s="10" t="s">
-        <v>7</v>
-      </c>
+      <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
-      <c r="M4" s="10" t="s">
-        <v>6</v>
-      </c>
+      <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
       <c r="P4" s="10"/>
@@ -747,17 +731,15 @@
     </row>
     <row r="5" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" s="9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>5</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -766,9 +748,7 @@
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
-      <c r="M5" s="10" t="s">
-        <v>6</v>
-      </c>
+      <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
       <c r="P5" s="10"/>
@@ -799,34 +779,24 @@
     </row>
     <row r="6" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" s="9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C6" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>6</v>
-      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>5</v>
-      </c>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
       <c r="L6" s="10"/>
-      <c r="M6" s="10" t="s">
-        <v>5</v>
-      </c>
+      <c r="M6" s="10"/>
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
@@ -857,32 +827,24 @@
     </row>
     <row r="7" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B7" s="9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="10"/>
-      <c r="E7" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-      <c r="H7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>5</v>
-      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
-      <c r="M7" s="10" t="s">
-        <v>5</v>
-      </c>
+      <c r="M7" s="10"/>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
@@ -913,13 +875,13 @@
     </row>
     <row r="8" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B8" s="9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C8" s="9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -930,9 +892,7 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
-      <c r="M8" s="10" t="s">
-        <v>5</v>
-      </c>
+      <c r="M8" s="10"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
       <c r="P8" s="10"/>
@@ -963,17 +923,15 @@
     </row>
     <row r="9" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B9" s="9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C9" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>6</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
@@ -982,9 +940,7 @@
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
-      <c r="M9" s="10" t="s">
-        <v>6</v>
-      </c>
+      <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
@@ -1015,30 +971,22 @@
     </row>
     <row r="10" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B10" s="12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C10" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>6</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D10" s="13"/>
       <c r="E10" s="13"/>
-      <c r="F10" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>

</xml_diff>

<commit_message>
Sikeres generálás! Értékelésnél egymás utáni műszakok, éjszakák és hétvégék számát veszi figyelembe.
</commit_message>
<xml_diff>
--- a/requests_admin.xlsx
+++ b/requests_admin.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Angyalka\python\Generalis\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="500"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Munka1" sheetId="1" r:id="rId1"/>
+    <sheet name="Munka1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -26,67 +22,85 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
   <si>
-    <t>Napok száma</t>
-  </si>
-  <si>
-    <t>Első szombat</t>
-  </si>
-  <si>
-    <t>Nappalos
+    <t xml:space="preserve">Napok száma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Első szombat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nappalos
 Műszakok #</t>
   </si>
   <si>
-    <t>Éjszakás
+    <t xml:space="preserve">Éjszakás
 Műszakok #</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>OUTSIDERS</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Bán Ádám</t>
-  </si>
-  <si>
-    <t>Gévay Kamilla</t>
-  </si>
-  <si>
-    <t>Mincsor-Szabó Orsolya</t>
-  </si>
-  <si>
-    <t>Baranyai Judit</t>
-  </si>
-  <si>
-    <t>Nédó Nóra</t>
-  </si>
-  <si>
-    <t>Muik Natasa</t>
-  </si>
-  <si>
-    <t>nx</t>
-  </si>
-  <si>
-    <t>éx</t>
-  </si>
-  <si>
-    <t>y</t>
+    <t xml:space="preserve">Bán Ádám</t>
+  </si>
+  <si>
+    <t xml:space="preserve">éx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gévay Kamilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mincsor-Szabó Orsolya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baranyai Judit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nédó Nóra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muik Natasa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUTSIDERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="7">
@@ -128,88 +142,119 @@
     </fill>
   </fills>
   <borders count="3">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="double">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="double"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -268,78 +313,62 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18A303"/>
+        <a:srgbClr val="18a303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369A3"/>
+        <a:srgbClr val="0369a3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A33E03"/>
+        <a:srgbClr val="a33e03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8E03A3"/>
+        <a:srgbClr val="8e03a3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="C99C00"/>
+        <a:srgbClr val="c99c00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="C9211E"/>
+        <a:srgbClr val="c9211e"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000EE"/>
+        <a:srgbClr val="0000ee"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551A8B"/>
+        <a:srgbClr val="551a8b"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -392,35 +421,36 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AN10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4:AG9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="13" style="1" customWidth="1"/>
-    <col min="4" max="40" width="3.7109375" style="1" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="4" style="1" width="3.71"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3">
+      <c r="B1" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="C1" s="4">
-        <f>SUM(B4:B10)</f>
+      <c r="C1" s="4" t="n">
+        <f aca="false">SUM(B4:B10)</f>
         <v>60</v>
       </c>
       <c r="D1" s="5"/>
@@ -461,15 +491,15 @@
       <c r="AM1" s="5"/>
       <c r="AN1" s="5"/>
     </row>
-    <row r="2" spans="1:40" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
-        <v>3</v>
-      </c>
-      <c r="C2" s="4">
-        <f>SUM(C4:C10)</f>
+      <c r="B2" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <f aca="false">SUM(C4:C10)</f>
         <v>30</v>
       </c>
       <c r="D2" s="5"/>
@@ -510,7 +540,7 @@
       <c r="AM2" s="5"/>
       <c r="AN2" s="5"/>
     </row>
-    <row r="3" spans="1:40" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
       <c r="B3" s="6" t="s">
         <v>2</v>
@@ -518,180 +548,180 @@
       <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="7">
-        <f t="shared" ref="E3:AN3" si="0">IF(D3="","",IF(D3+1-$B$1 &gt; 0, "", D3+1))</f>
+      <c r="E3" s="7" t="n">
+        <f aca="false">IF(D3="","",IF(D3+1-$B$1 &gt; 0, "", D3+1))</f>
         <v>2</v>
       </c>
-      <c r="F3" s="7">
-        <f t="shared" si="0"/>
+      <c r="F3" s="7" t="n">
+        <f aca="false">IF(E3="","",IF(E3+1-$B$1 &gt; 0, "", E3+1))</f>
         <v>3</v>
       </c>
-      <c r="G3" s="7">
-        <f t="shared" si="0"/>
+      <c r="G3" s="7" t="n">
+        <f aca="false">IF(F3="","",IF(F3+1-$B$1 &gt; 0, "", F3+1))</f>
         <v>4</v>
       </c>
-      <c r="H3" s="7">
-        <f t="shared" si="0"/>
+      <c r="H3" s="7" t="n">
+        <f aca="false">IF(G3="","",IF(G3+1-$B$1 &gt; 0, "", G3+1))</f>
         <v>5</v>
       </c>
-      <c r="I3" s="7">
-        <f t="shared" si="0"/>
+      <c r="I3" s="7" t="n">
+        <f aca="false">IF(H3="","",IF(H3+1-$B$1 &gt; 0, "", H3+1))</f>
         <v>6</v>
       </c>
-      <c r="J3" s="7">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="K3" s="7">
-        <f t="shared" si="0"/>
+      <c r="J3" s="7" t="n">
+        <f aca="false">IF(I3="","",IF(I3+1-$B$1 &gt; 0, "", I3+1))</f>
+        <v>7</v>
+      </c>
+      <c r="K3" s="7" t="n">
+        <f aca="false">IF(J3="","",IF(J3+1-$B$1 &gt; 0, "", J3+1))</f>
         <v>8</v>
       </c>
-      <c r="L3" s="7">
-        <f t="shared" si="0"/>
+      <c r="L3" s="7" t="n">
+        <f aca="false">IF(K3="","",IF(K3+1-$B$1 &gt; 0, "", K3+1))</f>
         <v>9</v>
       </c>
-      <c r="M3" s="7">
-        <f t="shared" si="0"/>
+      <c r="M3" s="7" t="n">
+        <f aca="false">IF(L3="","",IF(L3+1-$B$1 &gt; 0, "", L3+1))</f>
         <v>10</v>
       </c>
-      <c r="N3" s="7">
-        <f t="shared" si="0"/>
+      <c r="N3" s="7" t="n">
+        <f aca="false">IF(M3="","",IF(M3+1-$B$1 &gt; 0, "", M3+1))</f>
         <v>11</v>
       </c>
-      <c r="O3" s="7">
-        <f t="shared" si="0"/>
+      <c r="O3" s="7" t="n">
+        <f aca="false">IF(N3="","",IF(N3+1-$B$1 &gt; 0, "", N3+1))</f>
         <v>12</v>
       </c>
-      <c r="P3" s="7">
-        <f t="shared" si="0"/>
+      <c r="P3" s="7" t="n">
+        <f aca="false">IF(O3="","",IF(O3+1-$B$1 &gt; 0, "", O3+1))</f>
         <v>13</v>
       </c>
-      <c r="Q3" s="7">
-        <f t="shared" si="0"/>
+      <c r="Q3" s="7" t="n">
+        <f aca="false">IF(P3="","",IF(P3+1-$B$1 &gt; 0, "", P3+1))</f>
         <v>14</v>
       </c>
-      <c r="R3" s="7">
-        <f t="shared" si="0"/>
+      <c r="R3" s="7" t="n">
+        <f aca="false">IF(Q3="","",IF(Q3+1-$B$1 &gt; 0, "", Q3+1))</f>
         <v>15</v>
       </c>
-      <c r="S3" s="7">
-        <f t="shared" si="0"/>
+      <c r="S3" s="7" t="n">
+        <f aca="false">IF(R3="","",IF(R3+1-$B$1 &gt; 0, "", R3+1))</f>
         <v>16</v>
       </c>
-      <c r="T3" s="7">
-        <f t="shared" si="0"/>
+      <c r="T3" s="7" t="n">
+        <f aca="false">IF(S3="","",IF(S3+1-$B$1 &gt; 0, "", S3+1))</f>
         <v>17</v>
       </c>
-      <c r="U3" s="7">
-        <f t="shared" si="0"/>
+      <c r="U3" s="7" t="n">
+        <f aca="false">IF(T3="","",IF(T3+1-$B$1 &gt; 0, "", T3+1))</f>
         <v>18</v>
       </c>
-      <c r="V3" s="7">
-        <f t="shared" si="0"/>
+      <c r="V3" s="7" t="n">
+        <f aca="false">IF(U3="","",IF(U3+1-$B$1 &gt; 0, "", U3+1))</f>
         <v>19</v>
       </c>
-      <c r="W3" s="7">
-        <f t="shared" si="0"/>
+      <c r="W3" s="7" t="n">
+        <f aca="false">IF(V3="","",IF(V3+1-$B$1 &gt; 0, "", V3+1))</f>
         <v>20</v>
       </c>
-      <c r="X3" s="7">
-        <f t="shared" si="0"/>
+      <c r="X3" s="7" t="n">
+        <f aca="false">IF(W3="","",IF(W3+1-$B$1 &gt; 0, "", W3+1))</f>
         <v>21</v>
       </c>
-      <c r="Y3" s="7">
-        <f t="shared" si="0"/>
+      <c r="Y3" s="7" t="n">
+        <f aca="false">IF(X3="","",IF(X3+1-$B$1 &gt; 0, "", X3+1))</f>
         <v>22</v>
       </c>
-      <c r="Z3" s="7">
-        <f t="shared" si="0"/>
+      <c r="Z3" s="7" t="n">
+        <f aca="false">IF(Y3="","",IF(Y3+1-$B$1 &gt; 0, "", Y3+1))</f>
         <v>23</v>
       </c>
-      <c r="AA3" s="7">
-        <f t="shared" si="0"/>
+      <c r="AA3" s="7" t="n">
+        <f aca="false">IF(Z3="","",IF(Z3+1-$B$1 &gt; 0, "", Z3+1))</f>
         <v>24</v>
       </c>
-      <c r="AB3" s="7">
-        <f t="shared" si="0"/>
+      <c r="AB3" s="7" t="n">
+        <f aca="false">IF(AA3="","",IF(AA3+1-$B$1 &gt; 0, "", AA3+1))</f>
         <v>25</v>
       </c>
-      <c r="AC3" s="7">
-        <f t="shared" si="0"/>
+      <c r="AC3" s="7" t="n">
+        <f aca="false">IF(AB3="","",IF(AB3+1-$B$1 &gt; 0, "", AB3+1))</f>
         <v>26</v>
       </c>
-      <c r="AD3" s="7">
-        <f t="shared" si="0"/>
+      <c r="AD3" s="7" t="n">
+        <f aca="false">IF(AC3="","",IF(AC3+1-$B$1 &gt; 0, "", AC3+1))</f>
         <v>27</v>
       </c>
-      <c r="AE3" s="7">
-        <f t="shared" si="0"/>
+      <c r="AE3" s="7" t="n">
+        <f aca="false">IF(AD3="","",IF(AD3+1-$B$1 &gt; 0, "", AD3+1))</f>
         <v>28</v>
       </c>
-      <c r="AF3" s="7">
-        <f t="shared" si="0"/>
+      <c r="AF3" s="7" t="n">
+        <f aca="false">IF(AE3="","",IF(AE3+1-$B$1 &gt; 0, "", AE3+1))</f>
         <v>29</v>
       </c>
-      <c r="AG3" s="7">
-        <f t="shared" si="0"/>
+      <c r="AG3" s="7" t="n">
+        <f aca="false">IF(AF3="","",IF(AF3+1-$B$1 &gt; 0, "", AF3+1))</f>
         <v>30</v>
       </c>
       <c r="AH3" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f aca="false">IF(AG3="","",IF(AG3+1-$B$1 &gt; 0, "", AG3+1))</f>
         <v/>
       </c>
       <c r="AI3" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f aca="false">IF(AH3="","",IF(AH3+1-$B$1 &gt; 0, "", AH3+1))</f>
         <v/>
       </c>
       <c r="AJ3" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f aca="false">IF(AI3="","",IF(AI3+1-$B$1 &gt; 0, "", AI3+1))</f>
         <v/>
       </c>
       <c r="AK3" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f aca="false">IF(AJ3="","",IF(AJ3+1-$B$1 &gt; 0, "", AJ3+1))</f>
         <v/>
       </c>
       <c r="AL3" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f aca="false">IF(AK3="","",IF(AK3+1-$B$1 &gt; 0, "", AK3+1))</f>
         <v/>
       </c>
       <c r="AM3" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f aca="false">IF(AL3="","",IF(AL3+1-$B$1 &gt; 0, "", AL3+1))</f>
         <v/>
       </c>
       <c r="AN3" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f aca="false">IF(AM3="","",IF(AM3+1-$B$1 &gt; 0, "", AM3+1))</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:40" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="9">
+        <v>4</v>
+      </c>
+      <c r="B4" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="9" t="n">
         <v>6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="10" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
@@ -705,13 +735,13 @@
       <c r="V4" s="10"/>
       <c r="W4" s="10"/>
       <c r="X4" s="10" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="Y4" s="10"/>
       <c r="Z4" s="10"/>
       <c r="AA4" s="10"/>
       <c r="AB4" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC4" s="10"/>
       <c r="AD4" s="10"/>
@@ -726,24 +756,24 @@
       <c r="AM4" s="10"/>
       <c r="AN4" s="10"/>
     </row>
-    <row r="5" spans="1:40" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="9" t="n">
         <v>6</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
@@ -752,7 +782,7 @@
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
@@ -762,25 +792,25 @@
       <c r="U5" s="10"/>
       <c r="V5" s="10"/>
       <c r="W5" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="X5" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Y5" s="10"/>
       <c r="Z5" s="10"/>
       <c r="AA5" s="10"/>
       <c r="AB5" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="AC5" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AD5" s="10"/>
       <c r="AE5" s="10"/>
       <c r="AF5" s="10"/>
       <c r="AG5" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AH5" s="10"/>
       <c r="AI5" s="10"/>
@@ -790,21 +820,21 @@
       <c r="AM5" s="10"/>
       <c r="AN5" s="10"/>
     </row>
-    <row r="6" spans="1:40" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="9">
         <v>10</v>
       </c>
-      <c r="C6" s="9">
+      <c r="B6" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="C6" s="9" t="n">
         <v>6</v>
       </c>
       <c r="D6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>13</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
@@ -821,7 +851,7 @@
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U6" s="10"/>
       <c r="V6" s="10"/>
@@ -844,14 +874,14 @@
       <c r="AM6" s="10"/>
       <c r="AN6" s="10"/>
     </row>
-    <row r="7" spans="1:40" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="9">
+        <v>11</v>
+      </c>
+      <c r="B7" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="9" t="n">
         <v>6</v>
       </c>
       <c r="D7" s="10"/>
@@ -873,10 +903,10 @@
       <c r="T7" s="10"/>
       <c r="U7" s="10"/>
       <c r="V7" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="W7" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
@@ -896,14 +926,14 @@
       <c r="AM7" s="10"/>
       <c r="AN7" s="10"/>
     </row>
-    <row r="8" spans="1:40" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="9">
+        <v>12</v>
+      </c>
+      <c r="B8" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="9" t="n">
         <v>6</v>
       </c>
       <c r="D8" s="10"/>
@@ -944,14 +974,14 @@
       <c r="AM8" s="10"/>
       <c r="AN8" s="10"/>
     </row>
-    <row r="9" spans="1:40" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="9">
+        <v>13</v>
+      </c>
+      <c r="B9" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="9" t="n">
         <v>0</v>
       </c>
       <c r="D9" s="10"/>
@@ -971,10 +1001,10 @@
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U9" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
@@ -984,13 +1014,13 @@
       <c r="AA9" s="10"/>
       <c r="AB9" s="10"/>
       <c r="AC9" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AD9" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AE9" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AF9" s="10"/>
       <c r="AG9" s="10"/>
@@ -1002,14 +1032,14 @@
       <c r="AM9" s="10"/>
       <c r="AN9" s="10"/>
     </row>
-    <row r="10" spans="1:40" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="B10" s="12">
-        <v>5</v>
-      </c>
-      <c r="C10" s="12">
+      <c r="C10" s="12" t="n">
         <v>0</v>
       </c>
       <c r="D10" s="13"/>
@@ -1017,7 +1047,7 @@
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
@@ -1026,7 +1056,7 @@
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
       <c r="O10" s="13" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
@@ -1037,17 +1067,17 @@
       <c r="V10" s="13"/>
       <c r="W10" s="13"/>
       <c r="X10" s="13" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="Y10" s="13"/>
       <c r="Z10" s="13"/>
       <c r="AA10" s="13"/>
       <c r="AB10" s="13"/>
       <c r="AC10" s="13" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="AD10" s="13" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="AE10" s="13"/>
       <c r="AF10" s="13"/>
@@ -1061,7 +1091,12 @@
       <c r="AN10" s="13"/>
     </row>
   </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sikeres generálások, de a végső feltételek miatt stochasztikus működés.
</commit_message>
<xml_diff>
--- a/requests_admin.xlsx
+++ b/requests_admin.xlsx
@@ -66,7 +66,7 @@
     <t xml:space="preserve">Muik Natasa</t>
   </si>
   <si>
-    <t xml:space="preserve">OUTSIDERS</t>
+    <t xml:space="preserve">Külsősök</t>
   </si>
   <si>
     <t xml:space="preserve">n</t>
@@ -432,7 +432,7 @@
   <dimension ref="A1:AN10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4:AG9"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>